<commit_message>
last update with the assets
</commit_message>
<xml_diff>
--- a/AnualReportGenerator/Data/Config.xlsx
+++ b/AnualReportGenerator/Data/Config.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
-    <sheet name="Evaluation Warning" sheetId="12" r:id="rId4"/>
+    <sheet name="Evaluation Warning" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -95,6 +95,9 @@
     <t>ReportYear</t>
   </si>
   <si>
+    <t>AcmeLoginCredential</t>
+  </si>
+  <si>
     <t>MaxRetryNumber</t>
   </si>
   <si>
@@ -191,9 +194,6 @@
     <t>Asset</t>
   </si>
   <si>
-    <t>Credential</t>
-  </si>
-  <si>
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
@@ -203,19 +203,7 @@
     <t>AcmeWebsitLoginLink</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>The login link for Acme website</t>
-  </si>
-  <si>
-    <t>AcmeLoginCredential</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Login Credential to acme website</t>
   </si>
 </sst>
 </file>
@@ -565,8 +553,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A4">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578" defaultRowHeight="15" customHeight="1"/>
@@ -694,7 +682,14 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1"/>
@@ -1738,138 +1733,138 @@
     </row>
     <row r="2" ht="30">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" ht="45">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1"/>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1"/>
     <row r="17" ht="30">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -2850,17 +2845,16 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="C1">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85547" customWidth="1"/>
     <col min="2" max="2" width="30.14063" customWidth="1"/>
-    <col min="3" max="3" width="30.14063" customWidth="1"/>
-    <col min="4" max="4" width="60.28516" customWidth="1"/>
-    <col min="5" max="27" width="65.42578" customWidth="1"/>
+    <col min="3" max="3" width="60.28516" customWidth="1"/>
+    <col min="4" max="26" width="65.42578" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -2868,17 +2862,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -2900,7 +2892,6 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s">
@@ -2910,32 +2901,13 @@
         <v>59</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>64</v>
-      </c>
-    </row>
+    <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="14.25" customHeight="1"/>
     <row r="5" ht="14.25" customHeight="1"/>
     <row r="6" ht="14.25" customHeight="1"/>
@@ -3932,7 +3904,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
 </worksheet>
 </file>

</xml_diff>